<commit_message>
Bump to 0.8.0.  #21 - Add SheetListener, plus "before" callbacks for all listeners.  #23 - Allow ":" operator to separate cell references in formulas.  #26 - Escape "$" as "\$" so as not to evaluate such expressions; replace expressions individually to resolve rich text formatting bug with repeated expressions.
</commit_message>
<xml_diff>
--- a/jett-core/templates/CellListenerTemplate.xlsx
+++ b/jett-core/templates/CellListenerTemplate.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="CellListener" sheetId="1" r:id="rId1"/>
+    <sheet name="Before" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>The State of ${california.name}</t>
   </si>
@@ -97,6 +98,15 @@
   </si>
   <si>
     <t>${nevada.counties.fipsCode}</t>
+  </si>
+  <si>
+    <t>State Name:</t>
+  </si>
+  <si>
+    <t>Anything here; CellListener will replace!</t>
+  </si>
+  <si>
+    <t>The CellListener will replace the above content with ${california.name}</t>
   </si>
 </sst>
 </file>
@@ -666,4 +676,34 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>